<commit_message>
updated bifubc (covid), updated elec calibration
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/EoSEUwGDPiR/Elasticity of Sectoral Energy Use wrt Per Capita GDP in Recession.xlsx
+++ b/InputData/ctrl-settings/EoSEUwGDPiR/Elasticity of Sectoral Energy Use wrt Per Capita GDP in Recession.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\All_states_RMI\CA\ctrl-settings\EoSEUwGDPiR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\California\CA-eps\InputData\ctrl-settings\EoSEUwGDPiR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF327221-CDC5-4B42-A4E9-2720CD2B79A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F262D5-DEED-4BBD-A1A3-DC7F08772CC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="765" windowWidth="26355" windowHeight="16020" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4170" yWindow="630" windowWidth="24615" windowHeight="16635" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="343">
   <si>
     <t>About</t>
   </si>
@@ -1050,6 +1050,24 @@
   </si>
   <si>
     <t>California</t>
+  </si>
+  <si>
+    <t>(assume no change)</t>
+  </si>
+  <si>
+    <t>https://rhg.com/research/preliminary-us-emissions-2020/</t>
+  </si>
+  <si>
+    <t>assume 6% drop, Rhodium</t>
+  </si>
+  <si>
+    <t>assume 14.7% drop, Rhodium</t>
+  </si>
+  <si>
+    <t>assume 7% drop in emissions, rhodium</t>
+  </si>
+  <si>
+    <t>assume no change-Rhodium</t>
   </si>
 </sst>
 </file>
@@ -1099,7 +1117,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1124,6 +1142,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1139,7 +1163,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1179,6 +1203,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1657,10 +1683,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1674,27 +1700,30 @@
     <col min="7" max="7" width="87.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>331</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">
         <v>321</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>5</v>
       </c>
@@ -1707,7 +1736,7 @@
         <v>-2.5423728813559324E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>57</v>
       </c>
@@ -1720,7 +1749,7 @@
         <v>-6.892282294676029E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>56</v>
       </c>
@@ -1733,12 +1762,12 @@
         <v>-0.10839160839160844</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>5</v>
       </c>
@@ -1751,7 +1780,7 @@
         <v>2.3809523809523808E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>57</v>
       </c>
@@ -1762,7 +1791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>56</v>
       </c>
@@ -1775,12 +1804,12 @@
         <v>-8.0376538740043538E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>5</v>
       </c>
@@ -1793,7 +1822,7 @@
         <v>-5.6910569105691054E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>57</v>
       </c>
@@ -1805,7 +1834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>56</v>
       </c>
@@ -1842,18 +1871,15 @@
         <v>29</v>
       </c>
       <c r="B20">
-        <f>EIA!B12</f>
-        <v>19448</v>
+        <v>19092</v>
       </c>
       <c r="C20">
-        <f>EIA!C12</f>
-        <v>18423</v>
+        <v>18426</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
-        <f>-(1-C20/B20)</f>
-        <v>-5.2704648292883571E-2</v>
+        <v>-5.4812397246574003E-2</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>30</v>
@@ -1890,20 +1916,16 @@
         <v>6</v>
       </c>
       <c r="B26" s="6">
-        <f>SUMPRODUCT(B9:B11,C9:C11)/SUM(B9:B11)</f>
-        <v>-2.9839714430803268E-2</v>
+        <v>0</v>
       </c>
       <c r="C26" s="6">
-        <f>SUMPRODUCT(B14:B16,C14:C16)/SUM(B14:B16)</f>
-        <v>-7.2267902842862455E-2</v>
+        <v>-0.06</v>
       </c>
       <c r="D26" s="6">
-        <f>SUMPRODUCT(B4:B6,C4:C6)/SUM(B4:B6)</f>
-        <v>-8.9036114252317167E-2</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="E26" s="6">
-        <f>(EIA!C10-EIA!B10)/EIA!B10</f>
-        <v>-0.14242928452579035</v>
+        <v>-0.14699999999999999</v>
       </c>
       <c r="F26" s="13">
         <f>(EIA!C6-EIA!B6)/EIA!B6</f>
@@ -1920,26 +1942,41 @@
         <v>9</v>
       </c>
       <c r="B28" s="11">
-        <f>B26/$A$22</f>
-        <v>0.5661685524392801</v>
+        <v>0</v>
       </c>
       <c r="C28" s="11">
         <f>C26/$A$22</f>
-        <v>1.3711865116955995</v>
+        <v>1.0946428730363593</v>
       </c>
       <c r="D28" s="11">
         <f>D26/$A$22</f>
-        <v>1.689340829247868</v>
+        <v>1.2770833518757527</v>
       </c>
       <c r="E28" s="11">
         <f>E26/$A$22</f>
-        <v>2.7024046102025086</v>
+        <v>2.6818750389390802</v>
       </c>
       <c r="F28" s="11">
-        <f>F26/$A$22</f>
-        <v>0.34127117367817983</v>
+        <v>0</v>
       </c>
       <c r="G28" s="14"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>342</v>
+      </c>
+      <c r="C29" t="s">
+        <v>339</v>
+      </c>
+      <c r="D29" t="s">
+        <v>341</v>
+      </c>
+      <c r="E29" t="s">
+        <v>340</v>
+      </c>
+      <c r="F29" t="s">
+        <v>337</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1951,11 +1988,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AG181"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="1" max="1" width="50.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
@@ -2060,7 +2099,7 @@
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="27" t="s">
         <v>61</v>
       </c>
       <c r="B2" s="22">
@@ -2161,7 +2200,7 @@
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="27" t="s">
         <v>62</v>
       </c>
       <c r="B3" s="22">
@@ -2262,7 +2301,7 @@
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="28" t="s">
         <v>63</v>
       </c>
       <c r="B4">
@@ -2363,7 +2402,7 @@
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="27" t="s">
         <v>64</v>
       </c>
       <c r="B5" s="22">
@@ -2464,7 +2503,7 @@
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="27" t="s">
         <v>65</v>
       </c>
       <c r="B6" s="22">
@@ -2565,7 +2604,7 @@
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="27" t="s">
         <v>66</v>
       </c>
       <c r="B7" s="22">
@@ -8120,7 +8159,7 @@
       </c>
     </row>
     <row r="62" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A62" s="22" t="s">
+      <c r="A62" s="27" t="s">
         <v>121</v>
       </c>
       <c r="B62" s="22">
@@ -8221,7 +8260,7 @@
       </c>
     </row>
     <row r="63" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A63" s="22" t="s">
+      <c r="A63" s="27" t="s">
         <v>122</v>
       </c>
       <c r="B63" s="22">
@@ -8322,7 +8361,7 @@
       </c>
     </row>
     <row r="64" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="A64" s="28" t="s">
         <v>123</v>
       </c>
       <c r="B64">
@@ -8423,7 +8462,7 @@
       </c>
     </row>
     <row r="65" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A65" s="22" t="s">
+      <c r="A65" s="27" t="s">
         <v>124</v>
       </c>
       <c r="B65" s="22">
@@ -8524,7 +8563,7 @@
       </c>
     </row>
     <row r="66" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A66" s="22" t="s">
+      <c r="A66" s="27" t="s">
         <v>125</v>
       </c>
       <c r="B66" s="22">
@@ -8625,7 +8664,7 @@
       </c>
     </row>
     <row r="67" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A67" s="22" t="s">
+      <c r="A67" s="27" t="s">
         <v>126</v>
       </c>
       <c r="B67" s="22">
@@ -20248,9 +20287,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AG81"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="48" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -28443,7 +28487,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28706,7 +28750,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.140625" customWidth="1"/>
+    <col min="1" max="1" width="90" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -28723,7 +28767,7 @@
       </c>
       <c r="B2" s="7">
         <f>Calculations!E28</f>
-        <v>2.7024046102025086</v>
+        <v>2.6818750389390802</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -28732,7 +28776,7 @@
       </c>
       <c r="B3" s="14">
         <f>Calculations!F28</f>
-        <v>0.34127117367817983</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -28741,7 +28785,7 @@
       </c>
       <c r="B4" s="7">
         <f>Calculations!B28</f>
-        <v>0.5661685524392801</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -28750,7 +28794,7 @@
       </c>
       <c r="B5" s="7">
         <f>Calculations!C28</f>
-        <v>1.3711865116955995</v>
+        <v>1.0946428730363593</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -28758,8 +28802,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="7">
-        <f>Calculations!D28</f>
-        <v>1.689340829247868</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated elec demand for industry bifubc, ctrl settings take out commercial covid impact
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/EoSEUwGDPiR/Elasticity of Sectoral Energy Use wrt Per Capita GDP in Recession.xlsx
+++ b/InputData/ctrl-settings/EoSEUwGDPiR/Elasticity of Sectoral Energy Use wrt Per Capita GDP in Recession.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\California\CA-eps\InputData\ctrl-settings\EoSEUwGDPiR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B223E6-93A9-45B9-8086-BEFA90112781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7BAC796-5EBE-4B14-B0B0-6C93A7F1ACC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11355" yWindow="1695" windowWidth="16515" windowHeight="13785" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14325" yWindow="615" windowWidth="13515" windowHeight="16530" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -28691,7 +28691,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28739,8 +28739,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="7">
-        <f>Calculations!C28</f>
-        <v>1.3184590799370572</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated transp covid elasticity
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/EoSEUwGDPiR/Elasticity of Sectoral Energy Use wrt Per Capita GDP in Recession.xlsx
+++ b/InputData/ctrl-settings/EoSEUwGDPiR/Elasticity of Sectoral Energy Use wrt Per Capita GDP in Recession.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\California\CA-eps\InputData\ctrl-settings\EoSEUwGDPiR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7BAC796-5EBE-4B14-B0B0-6C93A7F1ACC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA2A935-F447-4C7A-B6CA-73A235E7E6B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14325" yWindow="615" windowWidth="13515" windowHeight="16530" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="337">
   <si>
     <t>About</t>
   </si>
@@ -1047,6 +1047,9 @@
   </si>
   <si>
     <t>Tables 5a, 6, 7a, and 9a</t>
+  </si>
+  <si>
+    <t>In California, covid adjustments are made in the inpud data files (bceu, bifubc, bcdtrsty)</t>
   </si>
 </sst>
 </file>
@@ -1458,10 +1461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1635,6 +1638,11 @@
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>328</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -28690,8 +28698,8 @@
   </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28712,8 +28720,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="7">
-        <f>Calculations!E28</f>
-        <v>2.5984866869637369</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>